<commit_message>
Dados atualizados pro MSI. Algoritmo que permite a comparacao de times de regioes distintas
</commit_message>
<xml_diff>
--- a/LCL_CIS_2019.xlsx
+++ b/LCL_CIS_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56BE9247-D9C8-4B9E-84BF-54FF0B33BF58}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59C5237-6D97-48BE-8880-5C9321D9BDD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="1500" windowWidth="17280" windowHeight="9420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All Games" sheetId="4" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="11">
   <si>
     <t>Winner</t>
   </si>
@@ -187,7 +187,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -216,6 +216,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -504,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C262"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B64"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,21 +1164,21 @@
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B59" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="7">
+      <c r="A59" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="6">
         <v>-1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B60" s="12" t="s">
+      <c r="A60" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C60" s="7">
@@ -1171,10 +1186,10 @@
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B61" s="12" t="s">
+      <c r="A61" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C61" s="7">
@@ -1182,10 +1197,10 @@
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C62" s="7">
@@ -1193,10 +1208,10 @@
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
+      <c r="A63" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="B63" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C63" s="7">
@@ -1204,77 +1219,105 @@
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A64" s="3" t="s">
+      <c r="A64" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C64" s="7">
         <v>-1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A65" s="3"/>
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A65" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B65" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A66" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A67" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" s="7">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B68" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C68" s="13">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="3"/>
       <c r="B69" s="3"/>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="3"/>
       <c r="B70" s="3"/>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="3"/>
       <c r="B71" s="3"/>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="3"/>
       <c r="B72" s="3"/>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="3"/>
       <c r="B73" s="3"/>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="3"/>
       <c r="B74" s="3"/>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="3"/>
       <c r="B75" s="3"/>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="3"/>
       <c r="B76" s="3"/>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="3"/>
       <c r="B77" s="3"/>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="3"/>
       <c r="B78" s="3"/>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="3"/>
       <c r="B79" s="3"/>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="3"/>
       <c r="B80" s="3"/>
     </row>

</xml_diff>